<commit_message>
deleted un needed scripts.
</commit_message>
<xml_diff>
--- a/src/FACAD/Product Cost File  Oct 2025-2026 final-V3.xlsx
+++ b/src/FACAD/Product Cost File  Oct 2025-2026 final-V3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccdg40926\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\E49JGK0I\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\plant-rates\plantrates\src\FACAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC27728F-8EB0-4D8E-9EFE-4D69A6D4C9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E75179C-8A0C-410A-8797-E1DDB17383C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost File" sheetId="1" r:id="rId1"/>
@@ -39,8 +39,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="122">
   <si>
     <t>X - HYDROPROP 40/80 BULK BAG</t>
   </si>
@@ -375,9 +397,6 @@
     <t>Facad</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -400,6 +419,15 @@
   </si>
   <si>
     <t>Sum</t>
+  </si>
+  <si>
+    <t>Facad General</t>
+  </si>
+  <si>
+    <t>Total Prod Volume:</t>
+  </si>
+  <si>
+    <t>Total Sales Volume</t>
   </si>
 </sst>
 </file>
@@ -407,12 +435,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
@@ -463,12 +491,23 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -491,7 +530,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -500,6 +538,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -818,20 +857,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" style="16" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>94</v>
       </c>
@@ -844,14 +883,14 @@
       <c r="E1" t="s">
         <v>107</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>108</v>
       </c>
       <c r="G1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>39</v>
       </c>
@@ -870,7 +909,7 @@
         <f>12.5/2.205</f>
         <v>5.6689342403628116</v>
       </c>
-      <c r="F2" s="17"/>
+      <c r="F2" s="16"/>
       <c r="G2" t="s">
         <v>89</v>
       </c>
@@ -881,7 +920,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
@@ -906,7 +945,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -931,7 +970,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
@@ -956,7 +995,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -982,7 +1021,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1002,7 +1041,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>100</v>
       </c>
@@ -1013,15 +1052,15 @@
       <c r="E8">
         <v>0.23300000000000001</v>
       </c>
-      <c r="F8" s="16">
-        <f>E8+'Operations Adder'!$H$5</f>
-        <v>0.27227920884049905</v>
+      <c r="F8" s="15">
+        <f>E8+'Operations Adder'!$I$5</f>
+        <v>0.25997576330604394</v>
       </c>
       <c r="G8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>72</v>
       </c>
@@ -1040,15 +1079,15 @@
         <f>0.2407+0.02</f>
         <v>0.26069999999999999</v>
       </c>
-      <c r="F9" s="16">
-        <f>E9+'Operations Adder'!$H$5</f>
-        <v>0.29997920884049906</v>
+      <c r="F9" s="15">
+        <f>E9+'Operations Adder'!$I$5</f>
+        <v>0.28767576330604389</v>
       </c>
       <c r="G9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>71</v>
       </c>
@@ -1067,15 +1106,15 @@
         <f>0.2407+0.02</f>
         <v>0.26069999999999999</v>
       </c>
-      <c r="F10" s="16">
-        <f>E10+'Operations Adder'!$H$5</f>
-        <v>0.29997920884049906</v>
+      <c r="F10" s="15">
+        <f>E10+'Operations Adder'!$I$5</f>
+        <v>0.28767576330604389</v>
       </c>
       <c r="G10" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>70</v>
       </c>
@@ -1094,15 +1133,15 @@
         <f>0.2795+0.02</f>
         <v>0.29950000000000004</v>
       </c>
-      <c r="F11" s="16">
-        <f>E11+'Operations Adder'!$H$5</f>
-        <v>0.33877920884049911</v>
+      <c r="F11" s="15">
+        <f>E11+'Operations Adder'!$I$5</f>
+        <v>0.32647576330604394</v>
       </c>
       <c r="G11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>69</v>
       </c>
@@ -1121,15 +1160,15 @@
         <f>0.2795+0.05</f>
         <v>0.32950000000000002</v>
       </c>
-      <c r="F12" s="16">
-        <f>E12+'Operations Adder'!$H$5</f>
-        <v>0.36877920884049908</v>
+      <c r="F12" s="15">
+        <f>E12+'Operations Adder'!$I$5</f>
+        <v>0.35647576330604391</v>
       </c>
       <c r="G12" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>66</v>
       </c>
@@ -1148,15 +1187,15 @@
         <f>0.2842+0.02</f>
         <v>0.30420000000000003</v>
       </c>
-      <c r="F13" s="16">
-        <f>E13+'Operations Adder'!$H$5</f>
-        <v>0.3434792088404991</v>
+      <c r="F13" s="15">
+        <f>E13+'Operations Adder'!$I$5</f>
+        <v>0.33117576330604392</v>
       </c>
       <c r="G13" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
@@ -1175,15 +1214,15 @@
         <f>0.2407+0.02</f>
         <v>0.26069999999999999</v>
       </c>
-      <c r="F14" s="16">
-        <f>E14+'Operations Adder'!$H$5</f>
-        <v>0.29997920884049906</v>
+      <c r="F14" s="15">
+        <f>E14+'Operations Adder'!$I$5</f>
+        <v>0.28767576330604389</v>
       </c>
       <c r="G14" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>58</v>
       </c>
@@ -1202,15 +1241,15 @@
         <f>0.2842+0.02</f>
         <v>0.30420000000000003</v>
       </c>
-      <c r="F15" s="16">
-        <f>E15+'Operations Adder'!$H$5</f>
-        <v>0.3434792088404991</v>
+      <c r="F15" s="15">
+        <f>E15+'Operations Adder'!$I$5</f>
+        <v>0.33117576330604392</v>
       </c>
       <c r="G15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>57</v>
       </c>
@@ -1229,15 +1268,15 @@
         <f>0.2407+0.05</f>
         <v>0.29070000000000001</v>
       </c>
-      <c r="F16" s="16">
-        <f>E16+'Operations Adder'!$H$5</f>
-        <v>0.32997920884049908</v>
+      <c r="F16" s="15">
+        <f>E16+'Operations Adder'!$I$5</f>
+        <v>0.31767576330604391</v>
       </c>
       <c r="G16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
@@ -1256,15 +1295,15 @@
         <f>0.2407+0.02</f>
         <v>0.26069999999999999</v>
       </c>
-      <c r="F17" s="16">
-        <f>E17+'Operations Adder'!$H$5</f>
-        <v>0.29997920884049906</v>
+      <c r="F17" s="15">
+        <f>E17+'Operations Adder'!$I$5</f>
+        <v>0.28767576330604389</v>
       </c>
       <c r="G17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>55</v>
       </c>
@@ -1283,15 +1322,15 @@
         <f>0.2432+0.02</f>
         <v>0.26319999999999999</v>
       </c>
-      <c r="F18" s="16">
-        <f>E18+'Operations Adder'!$H$5</f>
-        <v>0.30247920884049906</v>
+      <c r="F18" s="15">
+        <f>E18+'Operations Adder'!$I$5</f>
+        <v>0.29017576330604389</v>
       </c>
       <c r="G18" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
@@ -1310,15 +1349,15 @@
         <f>0.2432+0.05</f>
         <v>0.29320000000000002</v>
       </c>
-      <c r="F19" s="16">
-        <f>E19+'Operations Adder'!$H$5</f>
-        <v>0.33247920884049909</v>
+      <c r="F19" s="15">
+        <f>E19+'Operations Adder'!$I$5</f>
+        <v>0.32017576330604391</v>
       </c>
       <c r="G19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
@@ -1337,15 +1376,15 @@
         <f>0.2432+0.05</f>
         <v>0.29320000000000002</v>
       </c>
-      <c r="F20" s="16">
-        <f>E20+'Operations Adder'!$H$5</f>
-        <v>0.33247920884049909</v>
+      <c r="F20" s="15">
+        <f>E20+'Operations Adder'!$I$5</f>
+        <v>0.32017576330604391</v>
       </c>
       <c r="G20" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
@@ -1364,15 +1403,15 @@
         <f>0.2423+0.02</f>
         <v>0.26229999999999998</v>
       </c>
-      <c r="F21" s="16">
-        <f>E21+'Operations Adder'!$H$5</f>
-        <v>0.30157920884049905</v>
+      <c r="F21" s="15">
+        <f>E21+'Operations Adder'!$I$5</f>
+        <v>0.28927576330604388</v>
       </c>
       <c r="G21" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>49</v>
       </c>
@@ -1391,15 +1430,15 @@
         <f>0.2007+0.05</f>
         <v>0.25069999999999998</v>
       </c>
-      <c r="F22" s="16">
-        <f>E22+'Operations Adder'!$H$5</f>
-        <v>0.28997920884049905</v>
+      <c r="F22" s="15">
+        <f>E22+'Operations Adder'!$I$5</f>
+        <v>0.27767576330604388</v>
       </c>
       <c r="G22" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>48</v>
       </c>
@@ -1418,15 +1457,15 @@
         <f>0.2077+0.02</f>
         <v>0.22769999999999999</v>
       </c>
-      <c r="F23" s="16">
-        <f>E23+'Operations Adder'!$H$5</f>
-        <v>0.26697920884049903</v>
+      <c r="F23" s="15">
+        <f>E23+'Operations Adder'!$I$5</f>
+        <v>0.25467576330604391</v>
       </c>
       <c r="G23" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>47</v>
       </c>
@@ -1445,15 +1484,15 @@
         <f>0.2842+0.05</f>
         <v>0.3342</v>
       </c>
-      <c r="F24" s="16">
-        <f>E24+'Operations Adder'!$H$5</f>
-        <v>0.37347920884049907</v>
+      <c r="F24" s="15">
+        <f>E24+'Operations Adder'!$I$5</f>
+        <v>0.3611757633060439</v>
       </c>
       <c r="G24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
@@ -1472,15 +1511,15 @@
         <f>0.2842+0.02</f>
         <v>0.30420000000000003</v>
       </c>
-      <c r="F25" s="16">
-        <f>E25+'Operations Adder'!$H$5</f>
-        <v>0.3434792088404991</v>
+      <c r="F25" s="15">
+        <f>E25+'Operations Adder'!$I$5</f>
+        <v>0.33117576330604392</v>
       </c>
       <c r="G25" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
@@ -1499,15 +1538,15 @@
         <f>0.2432+0.05</f>
         <v>0.29320000000000002</v>
       </c>
-      <c r="F26" s="16">
-        <f>E26+'Operations Adder'!$H$5</f>
-        <v>0.33247920884049909</v>
+      <c r="F26" s="15">
+        <f>E26+'Operations Adder'!$I$5</f>
+        <v>0.32017576330604391</v>
       </c>
       <c r="G26" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>44</v>
       </c>
@@ -1526,15 +1565,15 @@
         <f>0.2432+0.05</f>
         <v>0.29320000000000002</v>
       </c>
-      <c r="F27" s="16">
-        <f>E27+'Operations Adder'!$H$5</f>
-        <v>0.33247920884049909</v>
+      <c r="F27" s="15">
+        <f>E27+'Operations Adder'!$I$5</f>
+        <v>0.32017576330604391</v>
       </c>
       <c r="G27" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>43</v>
       </c>
@@ -1553,15 +1592,15 @@
         <f>0.2432+0.02</f>
         <v>0.26319999999999999</v>
       </c>
-      <c r="F28" s="16">
-        <f>E28+'Operations Adder'!$H$5</f>
-        <v>0.30247920884049906</v>
+      <c r="F28" s="15">
+        <f>E28+'Operations Adder'!$I$5</f>
+        <v>0.29017576330604389</v>
       </c>
       <c r="G28" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
@@ -1580,15 +1619,15 @@
         <f>0.2432+0.05</f>
         <v>0.29320000000000002</v>
       </c>
-      <c r="F29" s="16">
-        <f>E29+'Operations Adder'!$H$5</f>
-        <v>0.33247920884049909</v>
+      <c r="F29" s="15">
+        <f>E29+'Operations Adder'!$I$5</f>
+        <v>0.32017576330604391</v>
       </c>
       <c r="G29" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
@@ -1607,15 +1646,15 @@
         <f>0.2432+0.02</f>
         <v>0.26319999999999999</v>
       </c>
-      <c r="F30" s="16">
-        <f>E30+'Operations Adder'!$H$5</f>
-        <v>0.30247920884049906</v>
+      <c r="F30" s="15">
+        <f>E30+'Operations Adder'!$I$5</f>
+        <v>0.29017576330604389</v>
       </c>
       <c r="G30" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
@@ -1634,15 +1673,15 @@
         <f>0.4556+0.02</f>
         <v>0.47560000000000002</v>
       </c>
-      <c r="F31" s="16">
-        <f>E31+'Operations Adder'!$H$5</f>
-        <v>0.51487920884049909</v>
+      <c r="F31" s="15">
+        <f>E31+'Operations Adder'!$I$5</f>
+        <v>0.50257576330604392</v>
       </c>
       <c r="G31" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -1660,15 +1699,15 @@
       <c r="E32">
         <v>0.28420000000000001</v>
       </c>
-      <c r="F32" s="16">
-        <f>E32+'Operations Adder'!$H$5</f>
-        <v>0.32347920884049908</v>
+      <c r="F32" s="15">
+        <f>E32+'Operations Adder'!$I$5</f>
+        <v>0.31117576330604391</v>
       </c>
       <c r="G32" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -1687,15 +1726,15 @@
         <f>0.2842+0.02</f>
         <v>0.30420000000000003</v>
       </c>
-      <c r="F33" s="16">
-        <f>E33+'Operations Adder'!$H$5</f>
-        <v>0.3434792088404991</v>
+      <c r="F33" s="15">
+        <f>E33+'Operations Adder'!$I$5</f>
+        <v>0.33117576330604392</v>
       </c>
       <c r="G33" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>13</v>
       </c>
@@ -1713,15 +1752,15 @@
         <f>0.5372</f>
         <v>0.53720000000000001</v>
       </c>
-      <c r="F34" s="16">
-        <f>E34+'Operations Adder'!$H$5</f>
-        <v>0.57647920884049908</v>
+      <c r="F34" s="15">
+        <f>E34+'Operations Adder'!$I$5</f>
+        <v>0.56417576330604391</v>
       </c>
       <c r="G34" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>12</v>
       </c>
@@ -1739,15 +1778,15 @@
         <f>0.5372</f>
         <v>0.53720000000000001</v>
       </c>
-      <c r="F35" s="16">
-        <f>E35+'Operations Adder'!$H$5</f>
-        <v>0.57647920884049908</v>
+      <c r="F35" s="15">
+        <f>E35+'Operations Adder'!$I$5</f>
+        <v>0.56417576330604391</v>
       </c>
       <c r="G35" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>11</v>
       </c>
@@ -1765,15 +1804,15 @@
         <f>0.5372+0.04+0.02</f>
         <v>0.59720000000000006</v>
       </c>
-      <c r="F36" s="16">
-        <f>E36+'Operations Adder'!$H$6</f>
-        <v>0.62839158369572645</v>
+      <c r="F36" s="15">
+        <f>E36+'Operations Adder'!$I$6</f>
+        <v>0.62339979202360174</v>
       </c>
       <c r="G36" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>10</v>
       </c>
@@ -1791,15 +1830,15 @@
         <f>0.7585+0.02</f>
         <v>0.77849999999999997</v>
       </c>
-      <c r="F37" s="16">
-        <f>E37+'Operations Adder'!$H$5</f>
-        <v>0.81777920884049904</v>
+      <c r="F37" s="15">
+        <f>E37+'Operations Adder'!$I$5</f>
+        <v>0.80547576330604387</v>
       </c>
       <c r="G37" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>5</v>
       </c>
@@ -1817,15 +1856,15 @@
         <f>0.9341</f>
         <v>0.93410000000000004</v>
       </c>
-      <c r="F38" s="16">
-        <f>E38+'Operations Adder'!$H$5</f>
-        <v>0.97337920884049911</v>
+      <c r="F38" s="15">
+        <f>E38+'Operations Adder'!$I$5</f>
+        <v>0.96107576330604394</v>
       </c>
       <c r="G38" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>4</v>
       </c>
@@ -1844,15 +1883,15 @@
         <f>0.4236+0.02</f>
         <v>0.44359999999999999</v>
       </c>
-      <c r="F39" s="16">
-        <f>E39+'Operations Adder'!$H$5</f>
-        <v>0.48287920884049906</v>
+      <c r="F39" s="15">
+        <f>E39+'Operations Adder'!$I$5</f>
+        <v>0.47057576330604389</v>
       </c>
       <c r="G39" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
@@ -1871,15 +1910,15 @@
         <f>0.4236+0.005</f>
         <v>0.42859999999999998</v>
       </c>
-      <c r="F40" s="16">
-        <f>E40+'Operations Adder'!$H$5</f>
-        <v>0.46787920884049905</v>
+      <c r="F40" s="15">
+        <f>E40+'Operations Adder'!$I$5</f>
+        <v>0.45557576330604388</v>
       </c>
       <c r="G40" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>83</v>
       </c>
@@ -1898,15 +1937,15 @@
         <f>0.3284+0.02</f>
         <v>0.34840000000000004</v>
       </c>
-      <c r="F41" s="16">
-        <f>E41+'Operations Adder'!$H$6</f>
-        <v>0.37959158369572643</v>
+      <c r="F41" s="15">
+        <f>E41+'Operations Adder'!$I$6</f>
+        <v>0.37459979202360166</v>
       </c>
       <c r="G41" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
@@ -1925,15 +1964,15 @@
         <f>0.4937+0.05</f>
         <v>0.54370000000000007</v>
       </c>
-      <c r="F42" s="16">
-        <f>E42+'Operations Adder'!$H$6</f>
-        <v>0.57489158369572646</v>
+      <c r="F42" s="15">
+        <f>E42+'Operations Adder'!$I$6</f>
+        <v>0.56989979202360175</v>
       </c>
       <c r="G42" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>81</v>
       </c>
@@ -1952,15 +1991,15 @@
         <f>0.4937+0.02</f>
         <v>0.51370000000000005</v>
       </c>
-      <c r="F43" s="16">
-        <f>E43+'Operations Adder'!$H$6</f>
-        <v>0.54489158369572643</v>
+      <c r="F43" s="15">
+        <f>E43+'Operations Adder'!$I$6</f>
+        <v>0.53989979202360172</v>
       </c>
       <c r="G43" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>80</v>
       </c>
@@ -1977,15 +2016,15 @@
         <f>0.4309</f>
         <v>0.43090000000000001</v>
       </c>
-      <c r="F44" s="16">
-        <f>E44+'Operations Adder'!$H$6</f>
-        <v>0.46209158369572639</v>
+      <c r="F44" s="15">
+        <f>E44+'Operations Adder'!$I$6</f>
+        <v>0.45709979202360163</v>
       </c>
       <c r="G44" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>79</v>
       </c>
@@ -2004,15 +2043,15 @@
         <f>0.4309+0.02</f>
         <v>0.45090000000000002</v>
       </c>
-      <c r="F45" s="16">
-        <f>E45+'Operations Adder'!$H$6</f>
-        <v>0.48209158369572641</v>
+      <c r="F45" s="15">
+        <f>E45+'Operations Adder'!$I$6</f>
+        <v>0.47709979202360164</v>
       </c>
       <c r="G45" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>78</v>
       </c>
@@ -2029,15 +2068,15 @@
         <f>0.3253</f>
         <v>0.32529999999999998</v>
       </c>
-      <c r="F46" s="16">
-        <f>E46+'Operations Adder'!$H$6</f>
-        <v>0.35649158369572637</v>
+      <c r="F46" s="15">
+        <f>E46+'Operations Adder'!$I$6</f>
+        <v>0.3514997920236016</v>
       </c>
       <c r="G46" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>77</v>
       </c>
@@ -2054,15 +2093,15 @@
         <f>0.3181</f>
         <v>0.31809999999999999</v>
       </c>
-      <c r="F47" s="16">
-        <f>E47+'Operations Adder'!$H$6</f>
-        <v>0.34929158369572638</v>
+      <c r="F47" s="15">
+        <f>E47+'Operations Adder'!$I$6</f>
+        <v>0.34429979202360161</v>
       </c>
       <c r="G47" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>76</v>
       </c>
@@ -2081,15 +2120,15 @@
         <f>0.3181+0.02</f>
         <v>0.33810000000000001</v>
       </c>
-      <c r="F48" s="16">
-        <f>E48+'Operations Adder'!$H$6</f>
-        <v>0.3692915836957264</v>
+      <c r="F48" s="15">
+        <f>E48+'Operations Adder'!$I$6</f>
+        <v>0.36429979202360163</v>
       </c>
       <c r="G48" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>75</v>
       </c>
@@ -2108,15 +2147,15 @@
         <f>0.381+0.02</f>
         <v>0.40100000000000002</v>
       </c>
-      <c r="F49" s="16">
-        <f>E49+'Operations Adder'!$H$6</f>
-        <v>0.43219158369572641</v>
+      <c r="F49" s="15">
+        <f>E49+'Operations Adder'!$I$6</f>
+        <v>0.42719979202360164</v>
       </c>
       <c r="G49" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>99</v>
       </c>
@@ -2128,15 +2167,15 @@
         <f>0.5216+0.02</f>
         <v>0.54159999999999997</v>
       </c>
-      <c r="F50" s="16">
-        <f>E50+'Operations Adder'!$H$6</f>
-        <v>0.57279158369572636</v>
+      <c r="F50" s="15">
+        <f>E50+'Operations Adder'!$I$6</f>
+        <v>0.56779979202360165</v>
       </c>
       <c r="G50" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>74</v>
       </c>
@@ -2155,15 +2194,15 @@
         <f>0.4266</f>
         <v>0.42659999999999998</v>
       </c>
-      <c r="F51" s="16">
-        <f>E51+'Operations Adder'!$H$6</f>
-        <v>0.45779158369572637</v>
+      <c r="F51" s="15">
+        <f>E51+'Operations Adder'!$I$6</f>
+        <v>0.4527997920236016</v>
       </c>
       <c r="G51" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>73</v>
       </c>
@@ -2182,15 +2221,15 @@
         <f>0.4266+0.02</f>
         <v>0.4466</v>
       </c>
-      <c r="F52" s="16">
-        <f>E52+'Operations Adder'!$H$6</f>
-        <v>0.47779158369572639</v>
+      <c r="F52" s="15">
+        <f>E52+'Operations Adder'!$I$6</f>
+        <v>0.47279979202360162</v>
       </c>
       <c r="G52" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>68</v>
       </c>
@@ -2209,15 +2248,15 @@
         <f>0.4483+0.02</f>
         <v>0.46829999999999999</v>
       </c>
-      <c r="F53" s="16">
-        <f>E53+'Operations Adder'!$H$6</f>
-        <v>0.49949158369572638</v>
+      <c r="F53" s="15">
+        <f>E53+'Operations Adder'!$I$6</f>
+        <v>0.49449979202360161</v>
       </c>
       <c r="G53" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>67</v>
       </c>
@@ -2236,15 +2275,15 @@
         <f>0.4483+0.02</f>
         <v>0.46829999999999999</v>
       </c>
-      <c r="F54" s="16">
-        <f>E54+'Operations Adder'!$H$6</f>
-        <v>0.49949158369572638</v>
+      <c r="F54" s="15">
+        <f>E54+'Operations Adder'!$I$6</f>
+        <v>0.49449979202360161</v>
       </c>
       <c r="G54" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>64</v>
       </c>
@@ -2263,15 +2302,15 @@
         <f>0.3969+0.02</f>
         <v>0.41689999999999999</v>
       </c>
-      <c r="F55" s="16">
-        <f>E55+'Operations Adder'!$H$6</f>
-        <v>0.44809158369572638</v>
+      <c r="F55" s="15">
+        <f>E55+'Operations Adder'!$I$6</f>
+        <v>0.44309979202360161</v>
       </c>
       <c r="G55" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>63</v>
       </c>
@@ -2290,15 +2329,15 @@
         <f>0.2933+0.05</f>
         <v>0.34329999999999999</v>
       </c>
-      <c r="F56" s="16">
-        <f>E56+'Operations Adder'!$H$6</f>
-        <v>0.37449158369572638</v>
+      <c r="F56" s="15">
+        <f>E56+'Operations Adder'!$I$6</f>
+        <v>0.36949979202360161</v>
       </c>
       <c r="G56" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>62</v>
       </c>
@@ -2317,15 +2356,15 @@
         <f>0.2933+0.02</f>
         <v>0.31330000000000002</v>
       </c>
-      <c r="F57" s="16">
-        <f>E57+'Operations Adder'!$H$6</f>
-        <v>0.34449158369572641</v>
+      <c r="F57" s="15">
+        <f>E57+'Operations Adder'!$I$6</f>
+        <v>0.33949979202360164</v>
       </c>
       <c r="G57" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>61</v>
       </c>
@@ -2344,15 +2383,15 @@
         <f>0.2933+0.02</f>
         <v>0.31330000000000002</v>
       </c>
-      <c r="F58" s="16">
-        <f>E58+'Operations Adder'!$H$6</f>
-        <v>0.34449158369572641</v>
+      <c r="F58" s="15">
+        <f>E58+'Operations Adder'!$I$6</f>
+        <v>0.33949979202360164</v>
       </c>
       <c r="G58" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>60</v>
       </c>
@@ -2371,15 +2410,15 @@
         <f>0.4945+0.02</f>
         <v>0.51449999999999996</v>
       </c>
-      <c r="F59" s="16">
-        <f>E59+'Operations Adder'!$H$6</f>
-        <v>0.54569158369572635</v>
+      <c r="F59" s="15">
+        <f>E59+'Operations Adder'!$I$6</f>
+        <v>0.54069979202360163</v>
       </c>
       <c r="G59" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
@@ -2398,15 +2437,15 @@
         <f>0.4483+0.02</f>
         <v>0.46829999999999999</v>
       </c>
-      <c r="F60" s="16">
-        <f>E60+'Operations Adder'!$H$6</f>
-        <v>0.49949158369572638</v>
+      <c r="F60" s="15">
+        <f>E60+'Operations Adder'!$I$6</f>
+        <v>0.49449979202360161</v>
       </c>
       <c r="G60" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>34</v>
       </c>
@@ -2425,15 +2464,15 @@
         <f>0.4483+0.02</f>
         <v>0.46829999999999999</v>
       </c>
-      <c r="F61" s="16">
-        <f>E61+'Operations Adder'!$H$6</f>
-        <v>0.49949158369572638</v>
+      <c r="F61" s="15">
+        <f>E61+'Operations Adder'!$I$6</f>
+        <v>0.49449979202360161</v>
       </c>
       <c r="G61" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>22</v>
       </c>
@@ -2452,15 +2491,15 @@
         <f>0.2933+0.05</f>
         <v>0.34329999999999999</v>
       </c>
-      <c r="F62" s="16">
-        <f>E62+'Operations Adder'!$H$6</f>
-        <v>0.37449158369572638</v>
+      <c r="F62" s="15">
+        <f>E62+'Operations Adder'!$I$6</f>
+        <v>0.36949979202360161</v>
       </c>
       <c r="G62" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>21</v>
       </c>
@@ -2479,15 +2518,15 @@
         <f>0.2933</f>
         <v>0.29330000000000001</v>
       </c>
-      <c r="F63" s="16">
-        <f>E63+'Operations Adder'!$H$6</f>
-        <v>0.32449158369572639</v>
+      <c r="F63" s="15">
+        <f>E63+'Operations Adder'!$I$6</f>
+        <v>0.31949979202360163</v>
       </c>
       <c r="G63" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>97</v>
       </c>
@@ -2503,15 +2542,15 @@
       <c r="E64" s="2">
         <v>0.32890000000000003</v>
       </c>
-      <c r="F64" s="16">
-        <f>E64+'Operations Adder'!$H$6</f>
-        <v>0.36009158369572641</v>
+      <c r="F64" s="15">
+        <f>E64+'Operations Adder'!$I$6</f>
+        <v>0.35509979202360165</v>
       </c>
       <c r="G64" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>98</v>
       </c>
@@ -2530,15 +2569,15 @@
         <f>0.3289+0.02</f>
         <v>0.34890000000000004</v>
       </c>
-      <c r="F65" s="16">
-        <f>E65+'Operations Adder'!$H$6</f>
-        <v>0.38009158369572643</v>
+      <c r="F65" s="15">
+        <f>E65+'Operations Adder'!$I$6</f>
+        <v>0.37509979202360166</v>
       </c>
       <c r="G65" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>2</v>
       </c>
@@ -2552,7 +2591,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>1</v>
       </c>
@@ -2567,7 +2606,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>20</v>
       </c>
@@ -2586,15 +2625,15 @@
         <f>0.9061+0.02</f>
         <v>0.92610000000000003</v>
       </c>
-      <c r="F68" s="16">
-        <f>E68+'Operations Adder'!$H$4</f>
-        <v>0.98834152732116398</v>
+      <c r="F68" s="15">
+        <f>E68+'Operations Adder'!$I$4</f>
+        <v>0.95200306722294092</v>
       </c>
       <c r="G68" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>19</v>
       </c>
@@ -2613,15 +2652,15 @@
         <f t="shared" ref="E69:E71" si="1">0.9061+0.02</f>
         <v>0.92610000000000003</v>
       </c>
-      <c r="F69" s="16">
-        <f>E69+'Operations Adder'!$H$4</f>
-        <v>0.98834152732116398</v>
+      <c r="F69" s="15">
+        <f>E69+'Operations Adder'!$I$4</f>
+        <v>0.95200306722294092</v>
       </c>
       <c r="G69" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>18</v>
       </c>
@@ -2640,15 +2679,15 @@
         <f t="shared" si="1"/>
         <v>0.92610000000000003</v>
       </c>
-      <c r="F70" s="16">
-        <f>E70+'Operations Adder'!$H$4</f>
-        <v>0.98834152732116398</v>
+      <c r="F70" s="15">
+        <f>E70+'Operations Adder'!$I$4</f>
+        <v>0.95200306722294092</v>
       </c>
       <c r="G70" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>17</v>
       </c>
@@ -2667,15 +2706,15 @@
         <f t="shared" si="1"/>
         <v>0.92610000000000003</v>
       </c>
-      <c r="F71" s="16">
-        <f>E71+'Operations Adder'!$H$4</f>
-        <v>0.98834152732116398</v>
+      <c r="F71" s="15">
+        <f>E71+'Operations Adder'!$I$4</f>
+        <v>0.95200306722294092</v>
       </c>
       <c r="G71" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>16</v>
       </c>
@@ -2693,15 +2732,15 @@
         <f>0.4442</f>
         <v>0.44419999999999998</v>
       </c>
-      <c r="F72" s="16">
-        <f>E72+'Operations Adder'!$H$4</f>
-        <v>0.50644152732116388</v>
+      <c r="F72" s="15">
+        <f>E72+'Operations Adder'!$I$4</f>
+        <v>0.47010306722294087</v>
       </c>
       <c r="G72" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>15</v>
       </c>
@@ -2720,15 +2759,15 @@
         <f>0.4442+0.02</f>
         <v>0.4642</v>
       </c>
-      <c r="F73" s="16">
-        <f>E73+'Operations Adder'!$H$4</f>
-        <v>0.52644152732116389</v>
+      <c r="F73" s="15">
+        <f>E73+'Operations Adder'!$I$4</f>
+        <v>0.49010306722294089</v>
       </c>
       <c r="G73" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>14</v>
       </c>
@@ -2747,15 +2786,15 @@
         <f>0.4442+0.02</f>
         <v>0.4642</v>
       </c>
-      <c r="F74" s="16">
-        <f>E74+'Operations Adder'!$H$4</f>
-        <v>0.52644152732116389</v>
+      <c r="F74" s="15">
+        <f>E74+'Operations Adder'!$I$4</f>
+        <v>0.49010306722294089</v>
       </c>
       <c r="G74" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>6</v>
       </c>
@@ -2774,15 +2813,15 @@
         <f>0.4905+0.02</f>
         <v>0.51049999999999995</v>
       </c>
-      <c r="F75" s="16">
-        <f>E75+'Operations Adder'!$H$4</f>
-        <v>0.5727415273211639</v>
+      <c r="F75" s="15">
+        <f>E75+'Operations Adder'!$I$4</f>
+        <v>0.53640306722294084</v>
       </c>
       <c r="G75" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>105</v>
       </c>
@@ -2793,15 +2832,15 @@
         <f>1.0108</f>
         <v>1.0107999999999999</v>
       </c>
-      <c r="F76" s="16">
-        <f>E76+'Operations Adder'!$H$4</f>
-        <v>1.0730415273211638</v>
+      <c r="F76" s="15">
+        <f>E76+'Operations Adder'!$I$4</f>
+        <v>1.0367030672229407</v>
       </c>
       <c r="G76" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>101</v>
       </c>
@@ -2811,15 +2850,15 @@
       <c r="E77">
         <v>0.68149999999999999</v>
       </c>
-      <c r="F77" s="16">
-        <f>E77+'Operations Adder'!$H$4</f>
-        <v>0.74374152732116394</v>
+      <c r="F77" s="15">
+        <f>E77+'Operations Adder'!$I$4</f>
+        <v>0.70740306722294088</v>
       </c>
       <c r="G77" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>102</v>
       </c>
@@ -2830,15 +2869,15 @@
         <f>0.6788</f>
         <v>0.67879999999999996</v>
       </c>
-      <c r="F78" s="16">
-        <f>E78+'Operations Adder'!$H$4</f>
-        <v>0.74104152732116391</v>
+      <c r="F78" s="15">
+        <f>E78+'Operations Adder'!$I$4</f>
+        <v>0.70470306722294085</v>
       </c>
       <c r="G78" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>103</v>
       </c>
@@ -2849,15 +2888,15 @@
         <f>0.6652</f>
         <v>0.66520000000000001</v>
       </c>
-      <c r="F79" s="16">
-        <f>E79+'Operations Adder'!$H$4</f>
-        <v>0.72744152732116396</v>
+      <c r="F79" s="15">
+        <f>E79+'Operations Adder'!$I$4</f>
+        <v>0.6911030672229409</v>
       </c>
       <c r="G79" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>54</v>
       </c>
@@ -2876,15 +2915,15 @@
         <f>0.1861/0.9+0.02</f>
         <v>0.22677777777777774</v>
       </c>
-      <c r="F80" s="16">
-        <f>E80+'Operations Adder'!$H$7</f>
-        <v>0.25047966192633681</v>
+      <c r="F80" s="15">
+        <f>E80+'Operations Adder'!$I$7</f>
+        <v>0.25319597572278729</v>
       </c>
       <c r="G80" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>53</v>
       </c>
@@ -2903,15 +2942,15 @@
         <f>0.1861+0.02</f>
         <v>0.20609999999999998</v>
       </c>
-      <c r="F81" s="16">
-        <f>E81+'Operations Adder'!$H$7</f>
-        <v>0.22980188414855904</v>
+      <c r="F81" s="15">
+        <f>E81+'Operations Adder'!$I$7</f>
+        <v>0.23251819794500955</v>
       </c>
       <c r="G81" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>31</v>
       </c>
@@ -2928,15 +2967,15 @@
       <c r="E82" s="2">
         <v>0.1971</v>
       </c>
-      <c r="F82" s="16">
-        <f>E82+'Operations Adder'!$H$7</f>
-        <v>0.22080188414855906</v>
+      <c r="F82" s="15">
+        <f>E82+'Operations Adder'!$I$7</f>
+        <v>0.22351819794500957</v>
       </c>
       <c r="G82" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>30</v>
       </c>
@@ -2955,15 +2994,15 @@
         <f>0.1971+0.02</f>
         <v>0.21709999999999999</v>
       </c>
-      <c r="F83" s="16">
-        <f>E83+'Operations Adder'!$H$7</f>
-        <v>0.24080188414855905</v>
+      <c r="F83" s="15">
+        <f>E83+'Operations Adder'!$I$7</f>
+        <v>0.24351819794500956</v>
       </c>
       <c r="G83" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>29</v>
       </c>
@@ -2981,15 +3020,15 @@
         <f>0.1861</f>
         <v>0.18609999999999999</v>
       </c>
-      <c r="F84" s="16">
-        <f>E84+'Operations Adder'!$H$7</f>
-        <v>0.20980188414855905</v>
+      <c r="F84" s="15">
+        <f>E84+'Operations Adder'!$I$7</f>
+        <v>0.21251819794500956</v>
       </c>
       <c r="G84" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>28</v>
       </c>
@@ -3008,15 +3047,15 @@
         <f>0.1861+0.05</f>
         <v>0.23609999999999998</v>
       </c>
-      <c r="F85" s="16">
-        <f>E85+'Operations Adder'!$H$7</f>
-        <v>0.25980188414855904</v>
+      <c r="F85" s="15">
+        <f>E85+'Operations Adder'!$I$7</f>
+        <v>0.26251819794500952</v>
       </c>
       <c r="G85" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>27</v>
       </c>
@@ -3035,15 +3074,15 @@
         <f>0.1861+0.02</f>
         <v>0.20609999999999998</v>
       </c>
-      <c r="F86" s="16">
-        <f>E86+'Operations Adder'!$H$7</f>
-        <v>0.22980188414855904</v>
+      <c r="F86" s="15">
+        <f>E86+'Operations Adder'!$I$7</f>
+        <v>0.23251819794500955</v>
       </c>
       <c r="G86" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>26</v>
       </c>
@@ -3061,15 +3100,15 @@
       <c r="E87" s="2">
         <v>0.18609999999999999</v>
       </c>
-      <c r="F87" s="16">
-        <f>E87+'Operations Adder'!$H$7</f>
-        <v>0.20980188414855905</v>
+      <c r="F87" s="15">
+        <f>E87+'Operations Adder'!$I$7</f>
+        <v>0.21251819794500956</v>
       </c>
       <c r="G87" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>25</v>
       </c>
@@ -3088,15 +3127,15 @@
         <f>0.1861+0.05</f>
         <v>0.23609999999999998</v>
       </c>
-      <c r="F88" s="16">
-        <f>E88+'Operations Adder'!$H$7</f>
-        <v>0.25980188414855904</v>
+      <c r="F88" s="15">
+        <f>E88+'Operations Adder'!$I$7</f>
+        <v>0.26251819794500952</v>
       </c>
       <c r="G88" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>24</v>
       </c>
@@ -3115,15 +3154,15 @@
         <f>0.1861+0.02</f>
         <v>0.20609999999999998</v>
       </c>
-      <c r="F89" s="16">
-        <f>E89+'Operations Adder'!$H$7</f>
-        <v>0.22980188414855904</v>
+      <c r="F89" s="15">
+        <f>E89+'Operations Adder'!$I$7</f>
+        <v>0.23251819794500955</v>
       </c>
       <c r="G89" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>23</v>
       </c>
@@ -3142,15 +3181,15 @@
         <f>0.1861+0.02</f>
         <v>0.20609999999999998</v>
       </c>
-      <c r="F90" s="16">
-        <f>E90+'Operations Adder'!$H$7</f>
-        <v>0.22980188414855904</v>
+      <c r="F90" s="15">
+        <f>E90+'Operations Adder'!$I$7</f>
+        <v>0.23251819794500955</v>
       </c>
       <c r="G90" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>9</v>
       </c>
@@ -3169,15 +3208,15 @@
         <f>0.1861</f>
         <v>0.18609999999999999</v>
       </c>
-      <c r="F91" s="16">
-        <f>E91+'Operations Adder'!$H$7</f>
-        <v>0.20980188414855905</v>
+      <c r="F91" s="15">
+        <f>E91+'Operations Adder'!$I$7</f>
+        <v>0.21251819794500956</v>
       </c>
       <c r="G91" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>8</v>
       </c>
@@ -3196,15 +3235,15 @@
         <f>0.1861+0.02</f>
         <v>0.20609999999999998</v>
       </c>
-      <c r="F92" s="16">
-        <f>E92+'Operations Adder'!$H$7</f>
-        <v>0.22980188414855904</v>
+      <c r="F92" s="15">
+        <f>E92+'Operations Adder'!$I$7</f>
+        <v>0.23251819794500955</v>
       </c>
       <c r="G92" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>0</v>
       </c>
@@ -3219,7 +3258,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>104</v>
       </c>
@@ -3229,15 +3268,15 @@
       <c r="E94">
         <v>0.17499999999999999</v>
       </c>
-      <c r="F94" s="16">
-        <f>E94+'Operations Adder'!$H$7</f>
-        <v>0.19870188414855905</v>
+      <c r="F94" s="15">
+        <f>E94+'Operations Adder'!$I$7</f>
+        <v>0.20141819794500956</v>
       </c>
       <c r="G94" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>106</v>
       </c>
@@ -3249,9 +3288,9 @@
         <f>0.3506+0.2239</f>
         <v>0.57450000000000001</v>
       </c>
-      <c r="F95" s="16">
-        <f>E95+'Operations Adder'!$H$7</f>
-        <v>0.59820188414855913</v>
+      <c r="F95" s="15">
+        <f>E95+'Operations Adder'!$I$7</f>
+        <v>0.60091819794500956</v>
       </c>
       <c r="G95" t="s">
         <v>85</v>
@@ -3270,23 +3309,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA671EF-B26E-4F69-99E2-5E44126B9373}">
-  <dimension ref="C3:H16"/>
+  <dimension ref="C3:I16"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
         <v>109</v>
       </c>
@@ -3294,13 +3333,16 @@
         <v>110</v>
       </c>
       <c r="G3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I3" t="s">
         <v>111</v>
       </c>
-      <c r="H3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>88</v>
       </c>
@@ -3310,146 +3352,191 @@
       <c r="E4" s="8">
         <v>13700000</v>
       </c>
-      <c r="F4" s="16">
-        <v>4.1786496350364966E-2</v>
-      </c>
-      <c r="G4" s="16">
-        <v>2.0455030970798961E-2</v>
-      </c>
-      <c r="H4" s="16">
-        <v>6.2241527321163927E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="F4" s="15">
+        <f>$D4/$E$14</f>
+        <v>1.8185933479462498E-3</v>
+      </c>
+      <c r="G4" s="15" cm="1">
+        <f t="array" ref="G4">SUM($D$8:$D$12/$E$14)</f>
+        <v>4.8037930048603827E-3</v>
+      </c>
+      <c r="H4" s="15">
+        <f>$D$13/$E$15</f>
+        <v>1.9280680870134254E-2</v>
+      </c>
+      <c r="I4" s="15">
+        <f>SUM(F4:H4)</f>
+        <v>2.5903067222940886E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>86</v>
       </c>
       <c r="D5" s="7">
         <v>910149</v>
       </c>
-      <c r="E5" s="8">
-        <v>48350000</v>
-      </c>
-      <c r="F5" s="16">
-        <v>1.8824177869700105E-2</v>
-      </c>
-      <c r="G5" s="16">
-        <v>2.0455030970798958E-2</v>
-      </c>
-      <c r="H5" s="16">
-        <v>3.9279208840499062E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="E5" s="17">
+        <v>43750000</v>
+      </c>
+      <c r="F5" s="15">
+        <f t="shared" ref="F5:F7" si="0">$D5/$E$14</f>
+        <v>2.8912894310492709E-3</v>
+      </c>
+      <c r="G5" s="15" cm="1">
+        <f t="array" ref="G5">SUM($D$8:$D$12/$E$14)</f>
+        <v>4.8037930048603827E-3</v>
+      </c>
+      <c r="H5" s="15">
+        <f t="shared" ref="H5:H16" si="1">$D$13/$E$15</f>
+        <v>1.9280680870134254E-2</v>
+      </c>
+      <c r="I5" s="15">
+        <f t="shared" ref="I5:I7" si="2">SUM(F5:H5)</f>
+        <v>2.6975763306043909E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>85</v>
       </c>
       <c r="D6" s="7">
         <v>665881</v>
       </c>
-      <c r="E6" s="8">
-        <v>62020000</v>
-      </c>
-      <c r="F6" s="16">
-        <v>1.0736552724927443E-2</v>
-      </c>
-      <c r="G6" s="16">
-        <v>2.0455030970798961E-2</v>
-      </c>
-      <c r="H6" s="16">
-        <v>3.1191583695726402E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="E6" s="17">
+        <v>56200000</v>
+      </c>
+      <c r="F6" s="15">
+        <f t="shared" si="0"/>
+        <v>2.1153181486070079E-3</v>
+      </c>
+      <c r="G6" s="15" cm="1">
+        <f t="array" ref="G6">SUM($D$8:$D$12/$E$14)</f>
+        <v>4.8037930048603827E-3</v>
+      </c>
+      <c r="H6" s="15">
+        <f t="shared" si="1"/>
+        <v>1.9280680870134254E-2</v>
+      </c>
+      <c r="I6" s="15">
+        <f t="shared" si="2"/>
+        <v>2.6199792023601644E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>87</v>
       </c>
       <c r="D7" s="7">
         <v>734633</v>
       </c>
-      <c r="E7" s="8">
-        <v>226260000</v>
-      </c>
-      <c r="F7" s="16">
-        <v>3.2468531777600988E-3</v>
-      </c>
-      <c r="G7" s="16">
-        <v>2.0455030970798965E-2</v>
-      </c>
-      <c r="H7" s="16">
-        <v>2.3701884148559064E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="E7" s="17">
+        <v>201140000</v>
+      </c>
+      <c r="F7" s="15">
+        <f t="shared" si="0"/>
+        <v>2.3337240700149306E-3</v>
+      </c>
+      <c r="G7" s="15" cm="1">
+        <f t="array" ref="G7">SUM($D$8:$D$12/$E$14)</f>
+        <v>4.8037930048603827E-3</v>
+      </c>
+      <c r="H7" s="15">
+        <f t="shared" si="1"/>
+        <v>1.9280680870134254E-2</v>
+      </c>
+      <c r="I7" s="15">
+        <f t="shared" si="2"/>
+        <v>2.6418197945009568E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="9">
+        <v>14184</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>113</v>
       </c>
-      <c r="D8" s="10">
-        <v>14184</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
+      <c r="D9" s="10">
+        <v>151129</v>
+      </c>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="11">
-        <v>151129</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C10" t="s">
+      <c r="D10" s="10">
+        <v>455159</v>
+      </c>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="11">
-        <v>455159</v>
-      </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C11" t="s">
+      <c r="D11" s="9">
+        <v>259133</v>
+      </c>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="10">
-        <v>259133</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C12" t="s">
+      <c r="D12" s="9">
+        <v>632581</v>
+      </c>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>117</v>
       </c>
-      <c r="D12" s="10">
-        <v>632581</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
+      <c r="D13" s="9">
+        <v>5653825</v>
+      </c>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="11">
+        <v>314790000</v>
+      </c>
+      <c r="G14" s="12">
+        <v>7166011</v>
+      </c>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E15" s="8">
+        <v>293237829</v>
+      </c>
+      <c r="G15" s="13">
+        <v>2883138</v>
+      </c>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
         <v>118</v>
       </c>
-      <c r="D13" s="10">
-        <v>5653825</v>
-      </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="E14" s="12">
-        <v>350330000</v>
-      </c>
-      <c r="G14" s="13">
-        <v>7166011</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="G15" s="14">
-        <v>2883138</v>
-      </c>
-    </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="F16" t="s">
-        <v>119</v>
-      </c>
-      <c r="G16" s="15">
+      <c r="G16" s="14">
         <v>10049149</v>
       </c>
+      <c r="H16" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>